<commit_message>
bugs de Close y Comboboxes corregidos (aun sin terminar la funcion CurrentData)
</commit_message>
<xml_diff>
--- a/Saves/Test2.xlsx
+++ b/Saves/Test2.xlsx
@@ -458,8 +458,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B2" t="n">
         <v>15</v>
@@ -572,7 +574,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>45</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">

</xml_diff>